<commit_message>
Fix bug with registration and import user from file
</commit_message>
<xml_diff>
--- a/public/userImportTemplate.xlsx
+++ b/public/userImportTemplate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -34,36 +34,6 @@
   </si>
   <si>
     <t>telephone</t>
-  </si>
-  <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>users</t>
-  </si>
-  <si>
-    <t>admin</t>
-  </si>
-  <si>
-    <t>some@ya.ru</t>
-  </si>
-  <si>
-    <t>user2</t>
-  </si>
-  <si>
-    <t>users2</t>
-  </si>
-  <si>
-    <t>somes@ya.ru</t>
-  </si>
-  <si>
-    <t>user3</t>
-  </si>
-  <si>
-    <t>users3</t>
-  </si>
-  <si>
-    <t>some1@ya.ru</t>
   </si>
   <si>
     <t>sdjfs</t>
@@ -103,7 +73,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -124,13 +94,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,12 +138,8 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -201,10 +160,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -234,73 +193,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="0" t="n">
-        <v>1111</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>80933088805</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1111</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>80933088805</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="0" t="n">
-        <v>1111</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="n">
-        <v>80933088805</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="some@ya.ru"/>
-    <hyperlink ref="E3" r:id="rId2" display="somes@ya.ru"/>
-    <hyperlink ref="E4" r:id="rId3" display="some1@ya.ru"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -329,50 +222,50 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add two lines in template file for user import
</commit_message>
<xml_diff>
--- a/public/userImportTemplate.xlsx
+++ b/public/userImportTemplate.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>telephone</t>
+  </si>
+  <si>
+    <t>singleDevice</t>
+  </si>
+  <si>
+    <t>deviceId</t>
   </si>
   <si>
     <t>sdjfs</t>
@@ -160,10 +166,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -191,6 +197,12 @@
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -222,50 +234,50 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bug with user import from excel file
</commit_message>
<xml_diff>
--- a/public/userImportTemplate.xlsx
+++ b/public/userImportTemplate.xlsx
@@ -33,7 +33,7 @@
     <t>email</t>
   </si>
   <si>
-    <t>telephone</t>
+    <t>phone</t>
   </si>
   <si>
     <t>singleDevice</t>
@@ -169,7 +169,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>